<commit_message>
chore: publish core IG 3.0.0
</commit_message>
<xml_diff>
--- a/ig/core/StructureDefinition-lpr3-Identifier.xlsx
+++ b/ig/core/StructureDefinition-lpr3-Identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.4.0</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-27T14:13:17+02:00</t>
+    <t>2025-09-24T12:42:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -453,7 +453,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-uuidv5:LPR3 episodeOfCare identifiers must conform to a UUIDv5 {value.matches('urn:uuid:[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[5][a-fA-F0-9]{3}-[89aAbB][a-fA-F0-9]{3}-[a-fA-F0-9]{12}')}</t>
+uuidv5:LPR3 episodeOfCare identifiers must conform to a UUIDv5 {matches('urn:uuid:[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[5][a-fA-F0-9]{3}-[89aAbB][a-fA-F0-9]{3}-[a-fA-F0-9]{12}')}</t>
   </si>
   <si>
     <t>CX.1 / EI.1</t>
@@ -823,44 +823,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.55078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.55078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.1640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.1640625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="10.83984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="22.921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="20.21875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="162.5078125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="143.54296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="44.3984375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="32.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="84.33984375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="37.421875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="60.5" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="137.703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="25.296875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="53.91015625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="123.23828125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="21.80859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
chore: publish core IG 3.0.0 (#35)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/core/StructureDefinition-lpr3-Identifier.xlsx
+++ b/ig/core/StructureDefinition-lpr3-Identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.4.0</t>
+    <t>3.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-27T14:13:17+02:00</t>
+    <t>2025-09-24T12:42:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -453,7 +453,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-uuidv5:LPR3 episodeOfCare identifiers must conform to a UUIDv5 {value.matches('urn:uuid:[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[5][a-fA-F0-9]{3}-[89aAbB][a-fA-F0-9]{3}-[a-fA-F0-9]{12}')}</t>
+uuidv5:LPR3 episodeOfCare identifiers must conform to a UUIDv5 {matches('urn:uuid:[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[5][a-fA-F0-9]{3}-[89aAbB][a-fA-F0-9]{3}-[a-fA-F0-9]{12}')}</t>
   </si>
   <si>
     <t>CX.1 / EI.1</t>
@@ -823,44 +823,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.55078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.55078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="12.3828125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.1640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.1640625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="10.83984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="22.921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="20.21875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="162.5078125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="143.54296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="44.3984375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="32.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="84.33984375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="37.421875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="60.5" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="137.703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="25.296875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="53.91015625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="123.23828125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="21.80859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
chore: publish core IG 3.0.1
</commit_message>
<xml_diff>
--- a/ig/core/StructureDefinition-lpr3-Identifier.xlsx
+++ b/ig/core/StructureDefinition-lpr3-Identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-24T12:42:36+00:00</t>
+    <t>2025-10-29T07:28:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -397,7 +397,7 @@
     <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type|4.0.1</t>
   </si>
   <si>
     <t>CX.5</t>
@@ -490,7 +490,7 @@
     <t>Identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -833,7 +833,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="20.21875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="24.74609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -848,7 +848,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="84.33984375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="37.421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="38.1484375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
chore: publish core IG 3.0.1 (#47)
Co-authored-by: sksMedcom <sksMedcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/core/StructureDefinition-lpr3-Identifier.xlsx
+++ b/ig/core/StructureDefinition-lpr3-Identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-24T12:42:36+00:00</t>
+    <t>2025-10-29T07:28:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -397,7 +397,7 @@
     <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type|4.0.1</t>
   </si>
   <si>
     <t>CX.5</t>
@@ -490,7 +490,7 @@
     <t>Identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -833,7 +833,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="20.21875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="24.74609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -848,7 +848,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="84.33984375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="37.421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="38.1484375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
chore: publish core IG 4.0.0
</commit_message>
<xml_diff>
--- a/ig/core/StructureDefinition-lpr3-Identifier.xlsx
+++ b/ig/core/StructureDefinition-lpr3-Identifier.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AM$10</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -30,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.1</t>
+    <t>4.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-29T07:28:01+00:00</t>
+    <t>2026-01-13T14:04:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -638,6 +641,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -982,7 +1000,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>30</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>86</v>
       </c>
@@ -1200,7 +1218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>93</v>
       </c>
@@ -1311,7 +1329,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>104</v>
       </c>
@@ -1424,7 +1442,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>116</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>126</v>
       </c>
@@ -1556,7 +1574,7 @@
         <v>87</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="I7" t="s" s="2">
         <v>76</v>
@@ -1650,7 +1668,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>137</v>
       </c>
@@ -1669,7 +1687,7 @@
         <v>87</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="I8" t="s" s="2">
         <v>76</v>
@@ -1761,7 +1779,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>146</v>
       </c>
@@ -1870,7 +1888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>153</v>
       </c>
@@ -1982,6 +2000,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AM10">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>